<commit_message>
added legend text file
</commit_message>
<xml_diff>
--- a/Clue/BoardLayout.xlsx
+++ b/Clue/BoardLayout.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="18876" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="38">
   <si>
     <t>W</t>
   </si>
@@ -127,6 +128,9 @@
   </si>
   <si>
     <t>Ballroom</t>
+  </si>
+  <si>
+    <t>Walkway</t>
   </si>
 </sst>
 </file>
@@ -558,31 +562,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12" customWidth="1"/>
   </cols>
@@ -1537,6 +1541,12 @@
       </c>
       <c r="X12" s="10" t="s">
         <v>17</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
@@ -2439,7 +2449,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2451,7 +2461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>